<commit_message>
update liberiaCoverageVillageForm XLSform and Xforms
</commit_message>
<xml_diff>
--- a/xlsform/liberiaCoverageVillageForm.xlsx
+++ b/xlsform/liberiaCoverageVillageForm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ernest/Documents/GitHub/liberiaS3Mforms/xlsform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38335CC-E09E-344F-A900-B467502DC188}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C229D0E-1804-0E41-9557-3841D79736BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="515">
   <si>
     <t>type</t>
   </si>
@@ -1471,16 +1471,7 @@
     <t xml:space="preserve">pulldata('greaterMonroviaSPlist',  'HH',  'index_key', ${segment}) </t>
   </si>
   <si>
-    <t>est_hh</t>
-  </si>
-  <si>
     <t>nsegment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pulldata('greaterMonroviaSPlist',  'snumber',  'index_key', ${segment}) </t>
-  </si>
-  <si>
-    <t>round(int(${est_hh})  div (20 div int(${nsegment})), 0)</t>
   </si>
   <si>
     <t>spDescription1</t>
@@ -1527,9 +1518,6 @@
     <t xml:space="preserve">pulldata('greaterMonroviaSPlist',  'vnumber',  'index_key', ${segment}) </t>
   </si>
   <si>
-    <t>round(int(${est_hh})  div (20 div int(${nvillage})), 0)</t>
-  </si>
-  <si>
     <t>spInterval2</t>
   </si>
   <si>
@@ -1549,6 +1537,54 @@
   </si>
   <si>
     <t xml:space="preserve">pulldata('greaterMonroviaSPlist', 'map',  'index_key', ${segment}) </t>
+  </si>
+  <si>
+    <t>randomStart1</t>
+  </si>
+  <si>
+    <t>once(int(${spInterval1} * random()) + 1)</t>
+  </si>
+  <si>
+    <t>The sampling interval for this village is:
+&lt;h4&gt;&lt;span style="color:red"&gt;${spInterval2}&lt;/span&gt;&lt;/h4&gt;
+The random starting point for this village is:
+&lt;h4&gt;&lt;span style="color:red"&gt;${randomStart2}&lt;/span&gt;&lt;/h4&gt;</t>
+  </si>
+  <si>
+    <t>once(int(${spInterval2} * random()) + 1)</t>
+  </si>
+  <si>
+    <t>randomStart2</t>
+  </si>
+  <si>
+    <t>The sampling interval for this segment is:
+&lt;h4&gt;&lt;span style="color:red"&gt;${spInterval1}&lt;/span&gt;&lt;/h4&gt;
+The random starting point for this segment is:
+&lt;h4&gt;&lt;span style="color:red"&gt;${randomStart1}&lt;/span&gt;&lt;/h4&gt;</t>
+  </si>
+  <si>
+    <t>Urban Montserrado</t>
+  </si>
+  <si>
+    <t>label::English (en)</t>
+  </si>
+  <si>
+    <t>est_hh1</t>
+  </si>
+  <si>
+    <t>round(int(${est_hh1})  div (20 div int(${nsegment})), 0)</t>
+  </si>
+  <si>
+    <t>est_hh2</t>
+  </si>
+  <si>
+    <t>Estimated number of households in the village</t>
+  </si>
+  <si>
+    <t>round(int(${est_hh2})  div (20 div int(${nvillage})), 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pulldata('greaterMonroviaSPlist', 'snumber',  'index_key', ${segment}) </t>
   </si>
   <si>
     <t>&lt;h4&gt;You are about to survey:&lt;/h4&gt;
@@ -1556,38 +1592,8 @@
 &lt;strong&gt;Segment/Village:&lt;/strong&gt; &lt;span style="color:red"&gt;${sname}&lt;/span&gt;
 &lt;strong&gt;Clan:&lt;/strong&gt; &lt;span style="color:red"&gt;${clan1}&lt;/span&gt;
 &lt;strong&gt;Estimated total population:&lt;/strong&gt; &lt;span style="color:red"&gt;${est_pop}&lt;/span&gt;
-&lt;strong&gt;Estimated number of households:&lt;/strong&gt; &lt;span style="color:red"&gt;${est_hh}&lt;/span&gt;
+&lt;strong&gt;Estimated number of households:&lt;/strong&gt; &lt;span style="color:red"&gt;${est_hh1}&lt;/span&gt;
 [LINK TO MAP](${map})</t>
-  </si>
-  <si>
-    <t>randomStart1</t>
-  </si>
-  <si>
-    <t>once(int(${spInterval1} * random()) + 1)</t>
-  </si>
-  <si>
-    <t>The sampling interval for this village is:
-&lt;h4&gt;&lt;span style="color:red"&gt;${spInterval2}&lt;/span&gt;&lt;/h4&gt;
-The random starting point for this village is:
-&lt;h4&gt;&lt;span style="color:red"&gt;${randomStart2}&lt;/span&gt;&lt;/h4&gt;</t>
-  </si>
-  <si>
-    <t>once(int(${spInterval2} * random()) + 1)</t>
-  </si>
-  <si>
-    <t>randomStart2</t>
-  </si>
-  <si>
-    <t>The sampling interval for this segment is:
-&lt;h4&gt;&lt;span style="color:red"&gt;${spInterval1}&lt;/span&gt;&lt;/h4&gt;
-The random starting point for this segment is:
-&lt;h4&gt;&lt;span style="color:red"&gt;${randomStart1}&lt;/span&gt;&lt;/h4&gt;</t>
-  </si>
-  <si>
-    <t>Urban Montserrado</t>
-  </si>
-  <si>
-    <t>label::English (en)</t>
   </si>
 </sst>
 </file>
@@ -2085,13 +2091,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ33"/>
+  <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -2115,7 +2121,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>2</v>
@@ -2215,7 +2221,7 @@
         <v>466</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>467</v>
@@ -5333,7 +5339,7 @@
         <v>310</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>479</v>
+        <v>508</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -6365,7 +6371,7 @@
         <v>310</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -6375,7 +6381,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="12" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -7397,10 +7403,10 @@
         <v>465</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>504</v>
+        <v>514</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -7409,11 +7415,11 @@
         <v>310</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C14" s="6"/>
       <c r="J14" s="12" t="s">
-        <v>481</v>
+        <v>513</v>
       </c>
     </row>
     <row r="15" spans="1:1024" ht="34">
@@ -7421,10 +7427,10 @@
         <v>310</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>482</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" spans="1:1024" ht="17">
@@ -7432,10 +7438,10 @@
         <v>310</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="255">
@@ -7443,10 +7449,10 @@
         <v>465</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="J17" s="6"/>
     </row>
@@ -7496,7 +7502,7 @@
         <v>466</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>467</v>
@@ -7507,7 +7513,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="14"/>
@@ -7515,29 +7521,30 @@
     </row>
     <row r="23" spans="1:12" ht="34">
       <c r="A23" s="3" t="s">
-        <v>310</v>
+        <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="J23" s="12" t="s">
-        <v>487</v>
-      </c>
-      <c r="K23" s="7"/>
+        <v>510</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="J23" s="6"/>
+      <c r="K23" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="34">
       <c r="A24" s="3" t="s">
         <v>310</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>486</v>
+        <v>302</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="5"/>
       <c r="J24" s="12" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="K24" s="7"/>
     </row>
@@ -7546,27 +7553,19 @@
         <v>310</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="5"/>
       <c r="J25" s="12" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:12" ht="289">
-      <c r="A26" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>493</v>
-      </c>
+    <row r="26" spans="1:12">
+      <c r="C26" s="6"/>
       <c r="D26" s="5"/>
-      <c r="J26" s="6"/>
+      <c r="J26" s="12"/>
       <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:12" ht="34">
@@ -7574,80 +7573,108 @@
         <v>310</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="C27" s="6"/>
+      <c r="D27" s="5"/>
       <c r="J27" s="12" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="34">
+        <v>489</v>
+      </c>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:12" ht="289">
       <c r="A28" s="3" t="s">
-        <v>310</v>
+        <v>465</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="17">
+        <v>486</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:12" ht="34">
       <c r="A29" s="3" t="s">
         <v>310</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="238">
+        <v>491</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="J29" s="12" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="34">
       <c r="A30" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="17">
+      <c r="A31" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="238">
+      <c r="A32" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>507</v>
-      </c>
-      <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="8" t="s">
+      <c r="B32" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="C32" s="6"/>
-      <c r="D32" s="5"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="7"/>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="3" t="s">
+      <c r="B33" s="8"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="C34" s="6"/>
+      <c r="D34" s="5"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K35" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -7665,7 +7692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F541"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -7689,7 +7716,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>19</v>
@@ -7698,7 +7725,7 @@
         <v>297</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -7709,7 +7736,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:6">

</xml_diff>